<commit_message>
ultima actualizacion. lo hice con mucho cariño.
</commit_message>
<xml_diff>
--- a/flujos_prueba/Funza/flujo_5_equipmentStatus/tables/tiposEquipos_FUNZA.xlsx
+++ b/flujos_prueba/Funza/flujo_5_equipmentStatus/tables/tiposEquipos_FUNZA.xlsx
@@ -469,10 +469,10 @@
         </is>
       </c>
       <c r="B2" s="1" t="n">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3">
@@ -482,10 +482,10 @@
         </is>
       </c>
       <c r="B3" s="1" t="n">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4">
@@ -495,10 +495,10 @@
         </is>
       </c>
       <c r="B4" s="1" t="n">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5">
@@ -521,10 +521,10 @@
         </is>
       </c>
       <c r="B6" s="1" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>